<commit_message>
Excel export from history is now possible
</commit_message>
<xml_diff>
--- a/src/main/resources/insulin.xlsx
+++ b/src/main/resources/insulin.xlsx
@@ -7,13 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="General" r:id="rId3" sheetId="1"/>
-    <sheet name="Indexes" r:id="rId4" sheetId="2"/>
+    <sheet name="30-04-2021" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
   <si>
     <t>Information id</t>
   </si>
@@ -75,7 +75,7 @@
     <t>Thyroglobulin</t>
   </si>
   <si>
-    <t>Male</t>
+    <t>Female</t>
   </si>
   <si>
     <t>-</t>
@@ -108,7 +108,64 @@
     <t>stumvoll2</t>
   </si>
   <si>
+    <t>spise</t>
+  </si>
+  <si>
+    <t>Insulin Resistance</t>
+  </si>
+  <si>
+    <t>≅6.61</t>
+  </si>
+  <si>
+    <t>loghoma</t>
+  </si>
+  <si>
+    <t>Prediabetes</t>
+  </si>
+  <si>
+    <t>1.0±0.64</t>
+  </si>
+  <si>
+    <t>homab</t>
+  </si>
+  <si>
+    <t>113.1±30.56</t>
+  </si>
+  <si>
+    <t>homa</t>
+  </si>
+  <si>
+    <t>0.5-1.4</t>
+  </si>
+  <si>
+    <t>revised</t>
+  </si>
+  <si>
+    <t>0.448±0.013</t>
+  </si>
+  <si>
     <t>stumvoll1</t>
+  </si>
+  <si>
+    <t>mcauley</t>
+  </si>
+  <si>
+    <t>&lt;5.8</t>
+  </si>
+  <si>
+    <t>belfiore</t>
+  </si>
+  <si>
+    <t>Insulin resistance</t>
+  </si>
+  <si>
+    <t>≅1</t>
+  </si>
+  <si>
+    <t>Healthy</t>
+  </si>
+  <si>
+    <t>avingon</t>
   </si>
 </sst>
 </file>
@@ -181,7 +238,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:V4"/>
+  <dimension ref="A1:V7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -291,16 +348,16 @@
         <v>22</v>
       </c>
       <c r="F2" t="n">
-        <v>99.0</v>
+        <v>100.008</v>
       </c>
       <c r="G2" t="n">
-        <v>134.0</v>
+        <v>115.002</v>
       </c>
       <c r="H2" t="n">
-        <v>144.0</v>
+        <v>109.998</v>
       </c>
       <c r="I2" t="n">
-        <v>121.5</v>
+        <v>104.5</v>
       </c>
       <c r="J2" t="n">
         <v>99.0</v>
@@ -309,19 +366,19 @@
         <v>24</v>
       </c>
       <c r="L2" t="n">
-        <v>55.0</v>
+        <v>45.0</v>
       </c>
       <c r="M2" t="n">
-        <v>60.0</v>
+        <v>50.0</v>
       </c>
       <c r="N2" t="n">
-        <v>65.0</v>
+        <v>52.0</v>
       </c>
       <c r="O2" t="n">
-        <v>57.5</v>
+        <v>50.0</v>
       </c>
       <c r="P2" t="n">
-        <v>50.0</v>
+        <v>48.0</v>
       </c>
       <c r="Q2" t="n">
         <v>80.0</v>
@@ -329,17 +386,17 @@
       <c r="R2" t="n">
         <v>180.0</v>
       </c>
-      <c r="S2" t="s">
-        <v>21</v>
-      </c>
-      <c r="T2" t="s">
-        <v>21</v>
+      <c r="S2" t="n">
+        <v>34.996</v>
+      </c>
+      <c r="T2" t="n">
+        <v>15.0</v>
       </c>
       <c r="U2" t="s">
         <v>21</v>
       </c>
-      <c r="V2" t="s">
-        <v>21</v>
+      <c r="V2" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="3">
@@ -357,16 +414,16 @@
         <v>23</v>
       </c>
       <c r="F3" t="n">
-        <v>5.5</v>
+        <v>5.555999999999999</v>
       </c>
       <c r="G3" t="n">
-        <v>7.444444444444444</v>
+        <v>6.388999999999999</v>
       </c>
       <c r="H3" t="n">
-        <v>8.0</v>
+        <v>6.111</v>
       </c>
       <c r="I3" t="n">
-        <v>6.75</v>
+        <v>5.81</v>
       </c>
       <c r="J3" t="n">
         <v>5.5</v>
@@ -375,19 +432,19 @@
         <v>25</v>
       </c>
       <c r="L3" t="n">
-        <v>330.0</v>
+        <v>270.0</v>
       </c>
       <c r="M3" t="n">
-        <v>360.0</v>
+        <v>300.0</v>
       </c>
       <c r="N3" t="n">
-        <v>390.0</v>
+        <v>312.0</v>
       </c>
       <c r="O3" t="n">
-        <v>345.0</v>
+        <v>300.0</v>
       </c>
       <c r="P3" t="n">
-        <v>300.0</v>
+        <v>288.0</v>
       </c>
       <c r="Q3" t="n">
         <v>80.0</v>
@@ -395,20 +452,153 @@
       <c r="R3" t="n">
         <v>180.0</v>
       </c>
-      <c r="S3" t="s">
-        <v>21</v>
-      </c>
-      <c r="T3" t="s">
-        <v>21</v>
+      <c r="S3" t="n">
+        <v>0.9049909490561159</v>
+      </c>
+      <c r="T3" t="n">
+        <v>5.25</v>
       </c>
       <c r="U3" t="s">
         <v>21</v>
       </c>
-      <c r="V3" t="s">
-        <v>21</v>
+      <c r="V3" t="n">
+        <v>25.0</v>
       </c>
     </row>
     <row r="4"/>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5" t="s">
+        <v>20</v>
+      </c>
+      <c r="D5" t="n">
+        <v>21.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="G5" t="n">
+        <v>100.0</v>
+      </c>
+      <c r="H5" t="n">
+        <v>115.0</v>
+      </c>
+      <c r="I5" t="n">
+        <v>102.5</v>
+      </c>
+      <c r="J5" t="n">
+        <v>90.0</v>
+      </c>
+      <c r="K5" t="s">
+        <v>24</v>
+      </c>
+      <c r="L5" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="M5" t="n">
+        <v>25.0</v>
+      </c>
+      <c r="N5" t="n">
+        <v>35.0</v>
+      </c>
+      <c r="O5" t="n">
+        <v>39.5</v>
+      </c>
+      <c r="P5" t="n">
+        <v>44.0</v>
+      </c>
+      <c r="Q5" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="R5" t="s">
+        <v>21</v>
+      </c>
+      <c r="S5" t="s">
+        <v>21</v>
+      </c>
+      <c r="T5" t="s">
+        <v>21</v>
+      </c>
+      <c r="U5" t="n">
+        <v>15.0</v>
+      </c>
+      <c r="V5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="G6" t="n">
+        <v>5.555555555555555</v>
+      </c>
+      <c r="H6" t="n">
+        <v>6.388888888888888</v>
+      </c>
+      <c r="I6" t="n">
+        <v>5.69</v>
+      </c>
+      <c r="J6" t="n">
+        <v>5.0</v>
+      </c>
+      <c r="K6" t="s">
+        <v>25</v>
+      </c>
+      <c r="L6" t="n">
+        <v>36.0</v>
+      </c>
+      <c r="M6" t="n">
+        <v>150.0</v>
+      </c>
+      <c r="N6" t="n">
+        <v>210.0</v>
+      </c>
+      <c r="O6" t="n">
+        <v>237.0</v>
+      </c>
+      <c r="P6" t="n">
+        <v>264.0</v>
+      </c>
+      <c r="Q6" t="n">
+        <v>80.0</v>
+      </c>
+      <c r="R6" t="s">
+        <v>21</v>
+      </c>
+      <c r="S6" t="s">
+        <v>21</v>
+      </c>
+      <c r="T6" t="s">
+        <v>21</v>
+      </c>
+      <c r="U6" t="n">
+        <v>0.16935</v>
+      </c>
+      <c r="V6" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
@@ -416,7 +606,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -425,7 +615,7 @@
     <col min="1" max="1" width="14.34375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.015625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="7.125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="10.5703125" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="16.9140625" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="13.90625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -475,16 +665,227 @@
         <v>31</v>
       </c>
       <c r="D3" t="n">
+        <f>600 * POWER(General!S3, 0.185) / POWER(General!V3, 0.2) / POWER(General!Q3 / POWER(General!R3 / 100, 2), 1.338)</f>
+        <v>0.0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B4"/>
+      <c r="C4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" t="n">
+        <f>LN((General!F3 * General!L2)/ 22.5)</f>
+        <v>0.0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B5"/>
+      <c r="C5" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" t="n">
+        <f>(20 * General!L2) / (General!F3 - 3.5)</f>
+        <v>0.0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B6"/>
+      <c r="C6" t="s">
+        <v>39</v>
+      </c>
+      <c r="D6" t="n">
+        <f>(General!F3 * General!L2)/ 22.5</f>
+        <v>0.0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B7"/>
+      <c r="C7" t="s">
+        <v>41</v>
+      </c>
+      <c r="D7" t="n">
+        <f>1.0 / (LN(General!F3) + LN(General!L2) + LN(General!T3))</f>
+        <v>0.0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>21</v>
+      </c>
+      <c r="F7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="n">
+        <v>1.0</v>
+      </c>
+      <c r="B8"/>
+      <c r="C8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" t="n">
         <f>0.222 - 0.00333 * General!Q3 / POWER(General!R3 / 100, 2) - 0.0000779 *General!P3 - 0.000422 * General!D2</f>
         <v>0.0</v>
       </c>
-      <c r="E3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" t="s">
-        <v>21</v>
-      </c>
-    </row>
+      <c r="E8" t="s">
+        <v>21</v>
+      </c>
+      <c r="F8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9"/>
+    <row r="10">
+      <c r="A10" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B10"/>
+      <c r="C10" t="s">
+        <v>44</v>
+      </c>
+      <c r="D10" t="n">
+        <f>EXP(2.63 - 0.28 * LN(General!L5) - 0.31 * LN(General!U6))</f>
+        <v>0.0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B11"/>
+      <c r="C11" t="s">
+        <v>46</v>
+      </c>
+      <c r="D11" t="n">
+        <f>2 / (((0.5 * General!F6 + General!H6 + General!J6) / 19.08) * ((0.5 * General!L5 + General!N5 + General!P5) / 104.0) + 1 )</f>
+        <v>0.0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B12"/>
+      <c r="C12" t="s">
+        <v>34</v>
+      </c>
+      <c r="D12" t="n">
+        <f>LN((General!F6 * General!L5)/ 22.5)</f>
+        <v>0.0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F12" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B13"/>
+      <c r="C13" t="s">
+        <v>37</v>
+      </c>
+      <c r="D13" t="n">
+        <f>(20 * General!L5) / (General!F6 - 3.5)</f>
+        <v>0.0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>21</v>
+      </c>
+      <c r="F13" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B14"/>
+      <c r="C14" t="s">
+        <v>39</v>
+      </c>
+      <c r="D14" t="n">
+        <f>(General!F6 * General!L5)/ 22.5</f>
+        <v>0.0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
+      </c>
+      <c r="F14" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="n">
+        <v>2.0</v>
+      </c>
+      <c r="B15"/>
+      <c r="C15" t="s">
+        <v>50</v>
+      </c>
+      <c r="D15" t="n">
+        <f>((0.137 * 100000000 /(General!F6 * General!L5 * 150/General!Q6)) + 100000000 /(General!J6 * General!P5 * 150/General!Q6)) / 2</f>
+        <v>0.0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>21</v>
+      </c>
+      <c r="F15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>

<commit_message>
Photo upload with optimisation
</commit_message>
<xml_diff>
--- a/src/main/resources/insulin.xlsx
+++ b/src/main/resources/insulin.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
   <si>
     <t>Information id</t>
   </si>
@@ -105,7 +105,13 @@
     <t>Normal range</t>
   </si>
   <si>
-    <t>ogis</t>
+    <t>belfiore</t>
+  </si>
+  <si>
+    <t>Healthy</t>
+  </si>
+  <si>
+    <t>≅1</t>
   </si>
   <si>
     <t>cederholm</t>
@@ -117,10 +123,7 @@
     <t>79±14</t>
   </si>
   <si>
-    <t>revised</t>
-  </si>
-  <si>
-    <t>0.448±0.013</t>
+    <t>avingon</t>
   </si>
 </sst>
 </file>
@@ -309,13 +312,13 @@
         <v>120.0</v>
       </c>
       <c r="H2" t="n">
-        <v>115.0</v>
+        <v>120.0</v>
       </c>
       <c r="I2" t="n">
-        <v>112.5</v>
+        <v>110.0</v>
       </c>
       <c r="J2" t="n">
-        <v>110.0</v>
+        <v>100.0</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
@@ -324,13 +327,13 @@
         <v>55.0</v>
       </c>
       <c r="M2" t="n">
-        <v>63.0</v>
+        <v>65.0</v>
       </c>
       <c r="N2" t="n">
-        <v>45.0</v>
+        <v>65.0</v>
       </c>
       <c r="O2" t="n">
-        <v>50.0</v>
+        <v>60.0</v>
       </c>
       <c r="P2" t="n">
         <v>55.0</v>
@@ -338,14 +341,14 @@
       <c r="Q2" t="n">
         <v>80.0</v>
       </c>
-      <c r="R2" t="n">
-        <v>180.0</v>
+      <c r="R2" t="s">
+        <v>21</v>
       </c>
       <c r="S2" t="s">
         <v>21</v>
       </c>
-      <c r="T2" t="n">
-        <v>55.0</v>
+      <c r="T2" t="s">
+        <v>21</v>
       </c>
       <c r="U2" t="s">
         <v>21</v>
@@ -375,13 +378,13 @@
         <v>6.666666666666666</v>
       </c>
       <c r="H3" t="n">
-        <v>6.388888888888888</v>
+        <v>6.666666666666666</v>
       </c>
       <c r="I3" t="n">
-        <v>6.25</v>
+        <v>6.11</v>
       </c>
       <c r="J3" t="n">
-        <v>6.111111111111111</v>
+        <v>5.555555555555555</v>
       </c>
       <c r="K3" t="s">
         <v>25</v>
@@ -390,13 +393,13 @@
         <v>330.0</v>
       </c>
       <c r="M3" t="n">
-        <v>378.0</v>
+        <v>390.0</v>
       </c>
       <c r="N3" t="n">
-        <v>270.0</v>
+        <v>390.0</v>
       </c>
       <c r="O3" t="n">
-        <v>300.0</v>
+        <v>360.0</v>
       </c>
       <c r="P3" t="n">
         <v>330.0</v>
@@ -404,14 +407,14 @@
       <c r="Q3" t="n">
         <v>80.0</v>
       </c>
-      <c r="R3" t="n">
-        <v>180.0</v>
+      <c r="R3" t="s">
+        <v>21</v>
       </c>
       <c r="S3" t="s">
         <v>21</v>
       </c>
-      <c r="T3" t="n">
-        <v>19.25</v>
+      <c r="T3" t="s">
+        <v>21</v>
       </c>
       <c r="U3" t="s">
         <v>21</v>
@@ -468,14 +471,14 @@
         <v>30</v>
       </c>
       <c r="D2" t="n">
-        <f>((( 0.0118 * (General!I3 - 90 * 0.05551) + 1) * (792 * (( 6.5 * (5.551 * 75 / (0.1640443958298 * POWER(General!Q3, 0.515) * POWER(0.01 * General!R3, 0.422))) - 10000 * (General!J3 - General!I3) / 30 ) / General!I3 + 4514 / General!F3 ) / (General!O3 - General!L3 + 1951))) + (SQRT(POWER((( 0.0118 * (General!I3 - 90 * 0.05551) + 1) * (792 * (( 6.5 * (5.551 * 75 / (0.1640443958298 * POWER(General!Q3, 0.515) * POWER(0.01 * General!R3, 0.422))) - 10000 * (General!J3 - General!I3) / 30 ) / General!I3 + 4514 / General!F3 ) / (General!O3 - General!L3 + 1951))), 2) + 4 * 0.0118 * 173 * (General!I3 - 90 * 0.05551) * (792 * (( 6.5 * (5.551 * 75 / (0.1640443958298 * POWER(General!Q3, 0.515) * POWER(0.01 * General!R3, 0.422))) - 10000 * (General!J3 - General!I3) / 30 ) / General!I3 + 4514 / General!F3 ) / (General!O3 - General!L3 + 1951))))) / 2</f>
+        <f>2 / (((0.5 * General!F3 + General!H3 + General!J3) / 19.08) * ((0.5 * General!L2 + General!N2 + General!P2) / 104.0) + 1 )</f>
         <v>0.0</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -484,17 +487,17 @@
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="n">
         <f>(75000 + (General!F3-General!J3)* 1.15 * 180 * 0.19 *General!Q3)/(120 * AVERAGE(General!F3:General!H3,General!J3)*LN(AVERAGE(General!L2:General!N2,General!P2)))</f>
         <v>0.0</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4">
@@ -503,17 +506,17 @@
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="D4" t="n">
-        <f>1.0 / (LN(General!F3) + LN(General!L2) + LN(General!T3))</f>
+        <f>((0.137 * 100000000 /(General!F3 * General!L2 * 150/General!Q3)) + 100000000 /(General!J3 * General!P2 * 150/General!Q3)) / 2</f>
         <v>0.0</v>
       </c>
       <c r="E4" t="s">
         <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5"/>

</xml_diff>

<commit_message>
Password checked against API
</commit_message>
<xml_diff>
--- a/src/main/resources/insulin.xlsx
+++ b/src/main/resources/insulin.xlsx
@@ -7,13 +7,13 @@
   </bookViews>
   <sheets>
     <sheet name="General" r:id="rId3" sheetId="1"/>
-    <sheet name="Indexes.xlsx" r:id="rId4" sheetId="2"/>
+    <sheet name="05-06-2021" r:id="rId4" sheetId="2"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="36">
   <si>
     <t>Information id</t>
   </si>
@@ -75,7 +75,7 @@
     <t>Thyroglobulin</t>
   </si>
   <si>
-    <t>M</t>
+    <t>Male</t>
   </si>
   <si>
     <t>-</t>
@@ -105,28 +105,22 @@
     <t>Normal range</t>
   </si>
   <si>
-    <t>stumvoll2</t>
-  </si>
-  <si>
-    <t>cederholm</t>
-  </si>
-  <si>
-    <t>Type two diabetes</t>
-  </si>
-  <si>
-    <t>79±14</t>
-  </si>
-  <si>
-    <t>matsuda</t>
-  </si>
-  <si>
-    <t>Insulin Resistance</t>
-  </si>
-  <si>
-    <t>&lt;4.3</t>
-  </si>
-  <si>
-    <t>stumvoll1</t>
+    <t>belfiore</t>
+  </si>
+  <si>
+    <t>Healthy</t>
+  </si>
+  <si>
+    <t>≅1</t>
+  </si>
+  <si>
+    <t>revised</t>
+  </si>
+  <si>
+    <t>0.448±0.013</t>
+  </si>
+  <si>
+    <t>avingon</t>
   </si>
 </sst>
 </file>
@@ -312,46 +306,46 @@
         <v>100.0</v>
       </c>
       <c r="G2" t="n">
-        <v>115.0</v>
+        <v>120.0</v>
       </c>
       <c r="H2" t="n">
-        <v>154.0</v>
+        <v>120.0</v>
       </c>
       <c r="I2" t="n">
-        <v>172.0</v>
+        <v>110.0</v>
       </c>
       <c r="J2" t="n">
-        <v>190.0</v>
+        <v>100.0</v>
       </c>
       <c r="K2" t="s">
         <v>24</v>
       </c>
       <c r="L2" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="M2" t="n">
+        <v>56.0</v>
+      </c>
+      <c r="N2" t="n">
         <v>55.0</v>
       </c>
-      <c r="M2" t="n">
-        <v>65.0</v>
-      </c>
-      <c r="N2" t="n">
+      <c r="O2" t="n">
+        <v>55.5</v>
+      </c>
+      <c r="P2" t="n">
         <v>56.0</v>
-      </c>
-      <c r="O2" t="n">
-        <v>60.0</v>
-      </c>
-      <c r="P2" t="n">
-        <v>64.0</v>
       </c>
       <c r="Q2" t="n">
         <v>80.0</v>
       </c>
-      <c r="R2" t="n">
-        <v>180.0</v>
+      <c r="R2" t="s">
+        <v>21</v>
       </c>
       <c r="S2" t="s">
         <v>21</v>
       </c>
-      <c r="T2" t="s">
-        <v>21</v>
+      <c r="T2" t="n">
+        <v>55.0</v>
       </c>
       <c r="U2" t="s">
         <v>21</v>
@@ -378,46 +372,46 @@
         <v>5.555555555555555</v>
       </c>
       <c r="G3" t="n">
-        <v>6.388888888888888</v>
+        <v>6.666666666666666</v>
       </c>
       <c r="H3" t="n">
-        <v>8.555555555555555</v>
+        <v>6.666666666666666</v>
       </c>
       <c r="I3" t="n">
-        <v>9.56</v>
+        <v>6.11</v>
       </c>
       <c r="J3" t="n">
-        <v>10.555555555555555</v>
+        <v>5.555555555555555</v>
       </c>
       <c r="K3" t="s">
         <v>25</v>
       </c>
       <c r="L3" t="n">
+        <v>336.0</v>
+      </c>
+      <c r="M3" t="n">
+        <v>336.0</v>
+      </c>
+      <c r="N3" t="n">
         <v>330.0</v>
       </c>
-      <c r="M3" t="n">
-        <v>390.0</v>
-      </c>
-      <c r="N3" t="n">
+      <c r="O3" t="n">
+        <v>333.0</v>
+      </c>
+      <c r="P3" t="n">
         <v>336.0</v>
-      </c>
-      <c r="O3" t="n">
-        <v>360.0</v>
-      </c>
-      <c r="P3" t="n">
-        <v>384.0</v>
       </c>
       <c r="Q3" t="n">
         <v>80.0</v>
       </c>
-      <c r="R3" t="n">
-        <v>180.0</v>
+      <c r="R3" t="s">
+        <v>21</v>
       </c>
       <c r="S3" t="s">
         <v>21</v>
       </c>
-      <c r="T3" t="s">
-        <v>21</v>
+      <c r="T3" t="n">
+        <v>19.25</v>
       </c>
       <c r="U3" t="s">
         <v>21</v>
@@ -434,7 +428,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -443,7 +437,7 @@
     <col min="1" max="1" width="14.34375" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.015625" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="7.125" customWidth="true" bestFit="true"/>
-    <col min="5" max="5" width="17.4765625" customWidth="true" bestFit="true"/>
+    <col min="5" max="5" width="10.5703125" customWidth="true" bestFit="true"/>
     <col min="6" max="6" width="13.90625" customWidth="true" bestFit="true"/>
   </cols>
   <sheetData>
@@ -474,14 +468,14 @@
         <v>30</v>
       </c>
       <c r="D2" t="n">
-        <f>0.156 - 0.0000459 * General!P3 - 0.000321 * General!L3 - 0.00541 * General!J3</f>
+        <f>2 / (((0.5 * General!F3 + General!H3 + General!J3) / 19.08) * ((0.5 * General!L2 + General!N2 + General!P2) / 104.0) + 1 )</f>
         <v>0.0</v>
       </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
     </row>
     <row r="3">
@@ -490,17 +484,17 @@
       </c>
       <c r="B3"/>
       <c r="C3" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="D3" t="n">
-        <f>(75000 + (General!F3-General!J3)* 1.15 * 180 * 0.19 *General!Q3)/(120 * AVERAGE(General!F3:General!H3,General!J3)*LN(AVERAGE(General!L2:General!N2,General!P2)))</f>
+        <f>1.0 / (LN(General!F3) + LN(General!L2) + LN(General!T3))</f>
         <v>0.0</v>
       </c>
       <c r="E3" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
     </row>
     <row r="4">
@@ -509,39 +503,20 @@
       </c>
       <c r="B4"/>
       <c r="C4" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="D4" t="n">
-        <f>10000 / (SQRT(General!F2) * General!L2 * AVERAGE(General!F2:General!H2,General!J2) * AVERAGE(General!L2:General!N2,General!P2))</f>
+        <f>((0.137 * 100000000 /(General!F3 * General!L2 * 150/General!Q3)) + 100000000 /(General!J3 * General!P2 * 150/General!Q3)) / 2</f>
         <v>0.0</v>
       </c>
       <c r="E4" t="s">
-        <v>35</v>
+        <v>21</v>
       </c>
       <c r="F4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="n">
-        <v>1.0</v>
-      </c>
-      <c r="B5"/>
-      <c r="C5" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" t="n">
-        <f>0.222 - 0.00333 * General!Q3 / POWER(General!R3 / 100, 2) - 0.0000779 *General!P3 - 0.000422 * General!D2</f>
-        <v>0.0</v>
-      </c>
-      <c r="E5" t="s">
-        <v>21</v>
-      </c>
-      <c r="F5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="6"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="5"/>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>